<commit_message>
Auto push 2023-03-19 22:45:45.38
</commit_message>
<xml_diff>
--- a/project/project.xlsx
+++ b/project/project.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>프로젝트명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,26 +76,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원가입, 수정, 탈퇴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공통모듈 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>현재상영작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>개봉예정작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예고편</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자모드 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -108,11 +92,171 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원관리, 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 통계, 추천</t>
+    <t>통합,테스트 및 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 테스트 및 정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이용자 권한과 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이용자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평론가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자는 기본 계정기능 + 이용자관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 상단 노출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 작성, 평점 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰 작성, 평점 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 등록, 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글관리, 리뷰,평점삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 추천, 통계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인덱스 민트색 63 255 218</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 소분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller 요청경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전달파라미터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>View</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비회원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰글 목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰글 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰글 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰글 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -120,178 +264,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>통합,테스트 및 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마지막 테스트 및 정리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이용자 권한과 기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비회원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이용자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>평론가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자는 기본 계정기능 + 이용자관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시판 조회</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰 상단 노출</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰 작성, 평점 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰 작성, 평점 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원관리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 등록, 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글관리, 리뷰,평점삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>영화 추천, 통계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인덱스 민트색 63 255 218</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능 소분류</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>controller 요청경로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전달파라미터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>View</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정보수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원탈퇴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비회원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사용자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰글 목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰글 상세보기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰글 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰글 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>리뷰글 삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>댓글 삭제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,6 +333,58 @@
   </si>
   <si>
     <t>관리자 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화리스트(상영작,예고작)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화검색(이름,태그)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판(페이징,답변,첨부파일)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점 등록, 수정, 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자게 글 작성, 수정, 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자게 댓글 작성, 수정, 삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원관리(제재)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인홈페이지 조정(컨텐츠 추천)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자유게시판 관리(삭제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평점관리(삭제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인,로그아웃, 정보수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입, 탈퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,7 +448,18 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -700,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G27"/>
+  <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -762,71 +797,104 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>22</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B33:C34 B38:C39 B25:C29 B30:B31">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -843,80 +911,80 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -966,171 +1034,171 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>